<commit_message>
Add recent accuracy to csv, fix filex blacklist
</commit_message>
<xml_diff>
--- a/Documents/Accuracy.xlsx
+++ b/Documents/Accuracy.xlsx
@@ -169,6 +169,12 @@
                 <c:pt idx="9">
                   <c:v>41692</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>41713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41736</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -207,6 +213,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -263,6 +275,12 @@
                 <c:pt idx="9">
                   <c:v>41692</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>41713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41736</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -301,6 +319,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -317,11 +341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82319616"/>
-        <c:axId val="82325888"/>
+        <c:axId val="82515840"/>
+        <c:axId val="82518016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="82319616"/>
+        <c:axId val="82515840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82325888"/>
+        <c:crossAx val="82518016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -365,7 +389,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82325888"/>
+        <c:axId val="82518016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -405,7 +429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82319616"/>
+        <c:crossAx val="82515840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -761,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,8 +825,12 @@
       <c r="M3" s="2">
         <v>0.85</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.92</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -846,8 +874,12 @@
       <c r="M4" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.05</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -887,6 +919,12 @@
       </c>
       <c r="M5" s="3">
         <v>41692</v>
+      </c>
+      <c r="N5" s="3">
+        <v>41713</v>
+      </c>
+      <c r="O5" s="3">
+        <v>41736</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>

</xml_diff>